<commit_message>
feat: update task filtering logic in reporteView; modify placeholder text in Buscar input
</commit_message>
<xml_diff>
--- a/frontend/public/Plantilla_Tareas.xlsx
+++ b/frontend/public/Plantilla_Tareas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EPRESP\Desktop\Seguimiento de Tareas V1\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A85D6D-2F52-4909-9B0B-9116785C278E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDC5271-BD88-4A34-89B7-C941E990A499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas" sheetId="1" r:id="rId1"/>
@@ -32,15 +32,6 @@
   </si>
   <si>
     <t>Agentes asignados</t>
-  </si>
-  <si>
-    <t>Tareas Completadas</t>
-  </si>
-  <si>
-    <t>Tareas Vencidas</t>
-  </si>
-  <si>
-    <t>Tareas Activas</t>
   </si>
   <si>
     <t>Ortografía</t>
@@ -75,6 +66,15 @@
   <si>
     <t>Falta de documentación adjunta</t>
   </si>
+  <si>
+    <t>Completada</t>
+  </si>
+  <si>
+    <t>Vencida</t>
+  </si>
+  <si>
+    <t>Activa</t>
+  </si>
 </sst>
 </file>
 
@@ -89,15 +89,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -105,24 +117,483 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -133,42 +604,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2E6F588-1F2A-406F-B840-31D6733E3E95}" name="Tabla1" displayName="Tabla1" ref="A1:E13" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E13" xr:uid="{C2E6F588-1F2A-406F-B840-31D6733E3E95}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FB1E0535-E59F-4873-971E-6A2847979C57}" name="Nombre de la tarea"/>
-    <tableColumn id="2" xr3:uid="{76C23390-1E12-4344-9723-DD80C7FEB28E}" name="Agentes asignados"/>
-    <tableColumn id="3" xr3:uid="{FD525182-BE1B-4172-B672-CD5E265B2A55}" name="Tareas Completadas"/>
-    <tableColumn id="4" xr3:uid="{BF12A54D-11EE-4E12-8F15-CE97C71C4ACE}" name="Tareas Vencidas"/>
-    <tableColumn id="5" xr3:uid="{C96DDFBE-39FD-4E22-A8E8-66C9C015CC26}" name="Tareas Activas"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DFB5B071-CAE5-4E5F-A0BC-89F61E75B540}" name="Tabla3" displayName="Tabla3" ref="A1:M64" totalsRowShown="0">
-  <autoFilter ref="A1:M64" xr:uid="{DFB5B071-CAE5-4E5F-A0BC-89F61E75B540}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D478635B-092A-47A3-B2C3-CA8CA7DE1D04}" name="Nombre de la tarea"/>
-    <tableColumn id="2" xr3:uid="{37238850-B88A-4A7E-AFA6-F26664456252}" name="Agentes asignados"/>
-    <tableColumn id="3" xr3:uid="{030B11F8-B911-4799-A3E6-637DE01C8606}" name="Ortografía"/>
-    <tableColumn id="4" xr3:uid="{37BBB24E-B7A2-488D-8135-6F6339BF3F9C}" name="Formato"/>
-    <tableColumn id="5" xr3:uid="{7D827E83-1331-433A-BF5B-1B686711CB4F}" name="Contenido"/>
-    <tableColumn id="6" xr3:uid="{0B13D49F-FB85-41FA-8336-FB7534313836}" name="Modificación de contenido"/>
-    <tableColumn id="7" xr3:uid="{EC126AE5-F735-4350-9AB4-29631906DF4C}" name="Redacción"/>
-    <tableColumn id="8" xr3:uid="{C2D7C923-09E4-4454-870E-CDE7FB25B01A}" name="Citas incorrectas"/>
-    <tableColumn id="9" xr3:uid="{25AC018B-BDEA-49C4-8AFE-0FCBA3E34254}" name="No corresponde a lo solicitado"/>
-    <tableColumn id="10" xr3:uid="{0D20C8BA-A56B-4E24-A3DB-40E29BB7368E}" name="Información incorrecta"/>
-    <tableColumn id="11" xr3:uid="{0FC85544-D49C-4579-B0F6-5F1BB33D5540}" name="Error de calculo"/>
-    <tableColumn id="12" xr3:uid="{A171B633-ADA0-460D-A4C0-1F937DC7FF26}" name="Tarea incompleta"/>
-    <tableColumn id="13" xr3:uid="{29FB5A1A-A455-4DF7-AEEF-1CAAF0EF6FCF}" name="Falta de documentación adjunta"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -434,104 +869,691 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="6" width="20.7109375" customWidth="1"/>
+    <col min="4" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6796E2E2-B8AE-42E6-B1AE-48A2EC17A1A4}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="25.7109375" customWidth="1"/>
+    <col min="1" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26" customWidth="1"/>
+    <col min="13" max="13" width="27.42578125" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="25"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="26"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="13"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="28"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="28"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="13"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="18"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="30"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="30"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="30"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="30"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="30"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="30"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="30"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="30"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="30"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="30"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="30"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="30"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="30"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="30"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="30"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="30"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="30"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="30"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="30"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="30"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="30"/>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="32"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>